<commit_message>
just uploading the results without standardScaler lib. It is beautiful result on 10 epoches.
</commit_message>
<xml_diff>
--- a/DatasetResults_MLP_SMOTE_April_24/Model_training_accuracy_and_evaluations_MLP_CardiacPrediction_(37079, 40)_Epoch_10.xlsx
+++ b/DatasetResults_MLP_SMOTE_April_24/Model_training_accuracy_and_evaluations_MLP_CardiacPrediction_(37079, 40)_Epoch_10.xlsx
@@ -434,14 +434,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t xml:space="preserve">           0       0.89      0.83      0.86      7115</t>
+          <t xml:space="preserve">           0       0.98      0.93      0.95      7115</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">           1       0.84      0.90      0.87      7114</t>
+          <t xml:space="preserve">           1       0.93      0.98      0.96      7114</t>
         </is>
       </c>
     </row>
@@ -451,21 +451,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">    accuracy                           0.87     14229</t>
+          <t xml:space="preserve">    accuracy                           0.95     14229</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t xml:space="preserve">   macro avg       0.87      0.87      0.87     14229</t>
+          <t xml:space="preserve">   macro avg       0.96      0.95      0.95     14229</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>weighted avg       0.87      0.87      0.87     14229</t>
+          <t>weighted avg       0.96      0.95      0.95     14229</t>
         </is>
       </c>
     </row>
@@ -488,52 +488,52 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>[0.7803665399551392</t>
+          <t>[0.8724017143249512</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.815876841545105</t>
+          <t xml:space="preserve"> 0.9084040522575378</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8339746594429016</t>
+          <t xml:space="preserve"> 0.9285224676132202</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8397905826568604</t>
+          <t xml:space="preserve"> 0.9432643055915833</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8465903997421265</t>
+          <t xml:space="preserve"> 0.9518036246299744</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8486637473106384</t>
+          <t xml:space="preserve"> 0.9595522880554199</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8527576923370361</t>
+          <t xml:space="preserve"> 0.9646302461624146</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8530915379524231</t>
+          <t xml:space="preserve"> 0.9695851802825928</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8567989468574524</t>
+          <t xml:space="preserve"> 0.9722734689712524</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 0.8590129017829895]</t>
+          <t xml:space="preserve"> 0.9751023650169373]</t>
         </is>
       </c>
     </row>

</xml_diff>